<commit_message>
Added some methods for Workbook, Worksheet, Format.
</commit_message>
<xml_diff>
--- a/testtest.xlsx
+++ b/testtest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="25">
   <si>
     <t>你好</t>
   </si>
@@ -44,6 +44,51 @@
   </si>
   <si>
     <t>03月28日</t>
+  </si>
+  <si>
+    <t>成都</t>
+  </si>
+  <si>
+    <t>天气状况</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>最低气温</t>
+  </si>
+  <si>
+    <t>最高气温</t>
+  </si>
+  <si>
+    <t>云量</t>
+  </si>
+  <si>
+    <t>绵阳</t>
+  </si>
+  <si>
+    <t>德阳</t>
+  </si>
+  <si>
+    <t>雅安</t>
   </si>
 </sst>
 </file>
@@ -67,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,12 +120,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I4"/>
+  <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,7 +478,453 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>